<commit_message>
add features for month report
</commit_message>
<xml_diff>
--- a/Result.xlsx
+++ b/Result.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VsProjects\FuquanPythonPlot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DDA10A4F-02A7-4A9D-9B66-1CC27986C810}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{43DD833C-724A-4359-8127-0180FD9D6F83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2625" windowWidth="28800" windowHeight="12975"/>
   </bookViews>
@@ -486,16 +486,16 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>338.83100000000002</v>
+        <v>338.90100000000001</v>
       </c>
       <c r="B2" s="1">
-        <v>250.39400000000001</v>
+        <v>250.501</v>
       </c>
       <c r="C2" s="1">
         <v>0</v>
       </c>
       <c r="D2" s="1">
-        <v>0</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="E2" s="1">
         <v>0</v>
@@ -513,30 +513,30 @@
         <v>0</v>
       </c>
       <c r="J2" s="1">
-        <v>150.036</v>
+        <v>150.07400000000001</v>
       </c>
       <c r="K2" s="1">
-        <v>170.18299999999999</v>
+        <v>169.79</v>
       </c>
       <c r="L2" s="1">
-        <v>239.965</v>
+        <v>240.47200000000001</v>
       </c>
       <c r="M2" s="1">
-        <v>208.93899999999999</v>
+        <v>209.846</v>
       </c>
       <c r="N2" s="1">
-        <v>144.768</v>
+        <v>144.875</v>
       </c>
       <c r="O2" s="1">
-        <v>129.542</v>
+        <v>129.816</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>338.58199999999999</v>
+        <v>338.58</v>
       </c>
       <c r="B3" s="1">
-        <v>250.261</v>
+        <v>242.41300000000001</v>
       </c>
       <c r="C3" s="1">
         <v>0</v>
@@ -560,22 +560,22 @@
         <v>0</v>
       </c>
       <c r="J3" s="1">
-        <v>149.697</v>
+        <v>149.66200000000001</v>
       </c>
       <c r="K3" s="1">
-        <v>169.977</v>
+        <v>169.458</v>
       </c>
       <c r="L3" s="1">
-        <v>239.65899999999999</v>
+        <v>239.96100000000001</v>
       </c>
       <c r="M3" s="1">
-        <v>208.69900000000001</v>
+        <v>209.24100000000001</v>
       </c>
       <c r="N3" s="1">
-        <v>142.78</v>
+        <v>144.52699999999999</v>
       </c>
       <c r="O3" s="1">
-        <v>129.077</v>
+        <v>129.548</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update ylims and yticklabelFormat
</commit_message>
<xml_diff>
--- a/Result.xlsx
+++ b/Result.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VsProjects\FuquanPythonPlot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\VsProjects\FuquanPythonPlot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{43DD833C-724A-4359-8127-0180FD9D6F83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{578F4D8F-AFAE-4336-AED8-7719EBF2B97E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2625" windowWidth="28800" windowHeight="12975"/>
+    <workbookView xWindow="7200" yWindow="1170" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="Result" sheetId="1" r:id="rId1"/>
@@ -486,96 +486,96 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>338.90100000000001</v>
+        <v>338</v>
       </c>
       <c r="B2" s="1">
-        <v>250.501</v>
+        <v>250</v>
       </c>
       <c r="C2" s="1">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D2" s="1">
-        <v>2.9000000000000001E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="E2" s="1">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="F2" s="1">
-        <v>0</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="G2" s="1">
         <v>0</v>
       </c>
       <c r="H2" s="1">
-        <v>0</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="I2" s="1">
-        <v>0</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="J2" s="1">
-        <v>150.07400000000001</v>
+        <v>150.203</v>
       </c>
       <c r="K2" s="1">
-        <v>169.79</v>
+        <v>170.042</v>
       </c>
       <c r="L2" s="1">
-        <v>240.47200000000001</v>
+        <v>251.34899999999999</v>
       </c>
       <c r="M2" s="1">
-        <v>209.846</v>
+        <v>222.51499999999999</v>
       </c>
       <c r="N2" s="1">
-        <v>144.875</v>
+        <v>148.73400000000001</v>
       </c>
       <c r="O2" s="1">
-        <v>129.816</v>
+        <v>130.364</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>338.58</v>
+        <v>160.92699999999999</v>
       </c>
       <c r="B3" s="1">
-        <v>242.41300000000001</v>
+        <v>250</v>
       </c>
       <c r="C3" s="1">
         <v>0</v>
       </c>
       <c r="D3" s="1">
-        <v>0</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="E3" s="1">
         <v>0</v>
       </c>
       <c r="F3" s="1">
-        <v>0</v>
+        <v>-1.2999999999999999E-2</v>
       </c>
       <c r="G3" s="1">
-        <v>0</v>
+        <v>-2.1999999999999999E-2</v>
       </c>
       <c r="H3" s="1">
-        <v>0</v>
+        <v>-7.0000000000000001E-3</v>
       </c>
       <c r="I3" s="1">
-        <v>0</v>
+        <v>-1.0999999999999999E-2</v>
       </c>
       <c r="J3" s="1">
-        <v>149.66200000000001</v>
+        <v>149.63800000000001</v>
       </c>
       <c r="K3" s="1">
-        <v>169.458</v>
+        <v>169.52799999999999</v>
       </c>
       <c r="L3" s="1">
-        <v>239.96100000000001</v>
+        <v>250.577</v>
       </c>
       <c r="M3" s="1">
-        <v>209.24100000000001</v>
+        <v>222.08799999999999</v>
       </c>
       <c r="N3" s="1">
-        <v>144.52699999999999</v>
+        <v>148.40600000000001</v>
       </c>
       <c r="O3" s="1">
-        <v>129.548</v>
+        <v>129.84100000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add more auto processing code
</commit_message>
<xml_diff>
--- a/Result.xlsx
+++ b/Result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\VsProjects\FuquanPythonPlot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{578F4D8F-AFAE-4336-AED8-7719EBF2B97E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{277EBD39-0403-49DE-9EEF-A231208DB080}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="1170" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="7905" yWindow="1170" windowWidth="17490" windowHeight="12240"/>
   </bookViews>
   <sheets>
     <sheet name="Result" sheetId="1" r:id="rId1"/>
@@ -486,96 +486,96 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>338</v>
+        <v>7.9000000000007703E-2</v>
       </c>
       <c r="B2" s="1">
-        <v>250</v>
+        <v>0.33400000000000302</v>
       </c>
       <c r="C2" s="1">
-        <v>0.01</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D2" s="1">
-        <v>2.8000000000000001E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="E2" s="1">
         <v>0.02</v>
       </c>
       <c r="F2" s="1">
-        <v>7.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="G2" s="1">
-        <v>0</v>
+        <v>-7.0000000000000001E-3</v>
       </c>
       <c r="H2" s="1">
-        <v>8.9999999999999993E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="I2" s="1">
-        <v>1.2999999999999999E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="J2" s="1">
-        <v>150.203</v>
+        <v>150.11600000000001</v>
       </c>
       <c r="K2" s="1">
-        <v>170.042</v>
+        <v>170.208</v>
       </c>
       <c r="L2" s="1">
-        <v>251.34899999999999</v>
+        <v>251.20400000000001</v>
       </c>
       <c r="M2" s="1">
-        <v>222.51499999999999</v>
+        <v>222.47300000000001</v>
       </c>
       <c r="N2" s="1">
-        <v>148.73400000000001</v>
+        <v>148.75700000000001</v>
       </c>
       <c r="O2" s="1">
-        <v>130.364</v>
+        <v>130.17099999999999</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>160.92699999999999</v>
+        <v>-6.7999999999997798E-2</v>
       </c>
       <c r="B3" s="1">
-        <v>250</v>
+        <v>-1.5999999999991101E-2</v>
       </c>
       <c r="C3" s="1">
-        <v>0</v>
+        <v>-1.2999999999999999E-2</v>
       </c>
       <c r="D3" s="1">
-        <v>2.5000000000000001E-2</v>
+        <v>-4.0000000000000001E-3</v>
       </c>
       <c r="E3" s="1">
-        <v>0</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F3" s="1">
-        <v>-1.2999999999999999E-2</v>
+        <v>-1.4999999999999999E-2</v>
       </c>
       <c r="G3" s="1">
         <v>-2.1999999999999999E-2</v>
       </c>
       <c r="H3" s="1">
-        <v>-7.0000000000000001E-3</v>
+        <v>-8.9999999999999993E-3</v>
       </c>
       <c r="I3" s="1">
         <v>-1.0999999999999999E-2</v>
       </c>
       <c r="J3" s="1">
-        <v>149.63800000000001</v>
+        <v>149.65299999999999</v>
       </c>
       <c r="K3" s="1">
-        <v>169.52799999999999</v>
+        <v>169.63</v>
       </c>
       <c r="L3" s="1">
-        <v>250.577</v>
+        <v>249.71199999999999</v>
       </c>
       <c r="M3" s="1">
-        <v>222.08799999999999</v>
+        <v>222.10499999999999</v>
       </c>
       <c r="N3" s="1">
-        <v>148.40600000000001</v>
+        <v>148.43700000000001</v>
       </c>
       <c r="O3" s="1">
-        <v>129.84100000000001</v>
+        <v>129.83199999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>